<commit_message>
add note to seasongroup sheet about the length of z being different to the number of seasons
</commit_message>
<xml_diff>
--- a/SimInputs.xlsx
+++ b/SimInputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815180DE-9620-4601-9A6E-6DF8EB472336}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFB9C66-238C-4BD7-A359-54527F1EB999}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AD2BC9D-DA3E-4CEE-AD10-2AFDEBF17CDA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6AD2BC9D-DA3E-4CEE-AD10-2AFDEBF17CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="SeasonGroup" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,40 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Michael Young (21512438)</author>
+  </authors>
+  <commentList>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{B72934FE-FF97-4992-AF8D-83568F9736B9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+All false but needs to exist so that the z axis matches the z axis everywhere else</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -77,13 +111,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -421,16 +468,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34ABF65C-ABFC-403A-BDA5-59CA472BAE8F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34ABF65C-ABFC-403A-BDA5-59CA472BAE8F}">
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1970</v>
       </c>
@@ -500,7 +547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -535,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1972</v>
       </c>
@@ -570,7 +617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1973</v>
       </c>
@@ -605,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1974</v>
       </c>
@@ -640,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -675,7 +722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -710,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1977</v>
       </c>
@@ -745,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1978</v>
       </c>
@@ -780,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1979</v>
       </c>
@@ -815,7 +862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1980</v>
       </c>
@@ -850,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1981</v>
       </c>
@@ -885,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1982</v>
       </c>
@@ -920,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1983</v>
       </c>
@@ -955,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1984</v>
       </c>
@@ -990,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1985</v>
       </c>
@@ -1025,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1986</v>
       </c>
@@ -1060,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1987</v>
       </c>
@@ -1095,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1988</v>
       </c>
@@ -1130,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1989</v>
       </c>
@@ -1165,7 +1212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1990</v>
       </c>
@@ -1200,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1991</v>
       </c>
@@ -1235,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1992</v>
       </c>
@@ -1270,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1993</v>
       </c>
@@ -1305,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1994</v>
       </c>
@@ -1340,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1995</v>
       </c>
@@ -1375,7 +1422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1996</v>
       </c>
@@ -1410,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1997</v>
       </c>
@@ -1445,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1998</v>
       </c>
@@ -1480,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1999</v>
       </c>
@@ -1515,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2000</v>
       </c>
@@ -1550,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2001</v>
       </c>
@@ -1585,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2002</v>
       </c>
@@ -1620,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2003</v>
       </c>
@@ -1655,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2004</v>
       </c>
@@ -1690,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2005</v>
       </c>
@@ -1725,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2006</v>
       </c>
@@ -1760,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2007</v>
       </c>
@@ -1795,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2008</v>
       </c>
@@ -1830,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2009</v>
       </c>
@@ -1865,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2010</v>
       </c>
@@ -1900,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -1935,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2012</v>
       </c>
@@ -1970,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2013</v>
       </c>
@@ -2005,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2014</v>
       </c>
@@ -2040,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2015</v>
       </c>
@@ -2075,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2016</v>
       </c>
@@ -2110,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2017</v>
       </c>
@@ -2145,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2018</v>
       </c>
@@ -2180,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2019</v>
       </c>
@@ -2217,6 +2264,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2226,7 +2274,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2240,7 +2288,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>